<commit_message>
backend - create model and migration
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>password</t>
   </si>
@@ -42,9 +42,6 @@
     <t>product</t>
   </si>
   <si>
-    <t>uid</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -72,16 +69,10 @@
     <t>bill</t>
   </si>
   <si>
-    <t>cartId</t>
-  </si>
-  <si>
     <t>itemsInCart</t>
   </si>
   <si>
     <t>total</t>
-  </si>
-  <si>
-    <t>cart</t>
   </si>
   <si>
     <t>category</t>
@@ -486,7 +477,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,28 +495,28 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -534,13 +525,11 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H2" s="6"/>
       <c r="K2" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -549,13 +538,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
         <v>9</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -564,13 +553,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -579,22 +568,22 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -603,84 +592,77 @@
         <v>5</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E10" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="6"/>
+      <c r="E12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="H14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -688,15 +670,15 @@
         <v>3</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
@@ -706,17 +688,17 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>